<commit_message>
#32 多语言 1、body 空的不输出 snippet 2、markdown不采用mul lan输出
</commit_message>
<xml_diff>
--- a/tool/mul_lan_snippets/config/excel/mul_lan.xlsx
+++ b/tool/mul_lan_snippets/config/excel/mul_lan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="101">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -164,10 +164,6 @@
 {
         System.Console.WriteLine("Hello World\r");
 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>markdown</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -800,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -813,11 +809,10 @@
     <col min="5" max="5" width="64.75" customWidth="1"/>
     <col min="6" max="6" width="71.375" customWidth="1"/>
     <col min="7" max="7" width="57.125" customWidth="1"/>
-    <col min="8" max="8" width="25.75" customWidth="1"/>
-    <col min="9" max="9" width="27.875" customWidth="1"/>
+    <col min="8" max="8" width="27.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -840,13 +835,10 @@
         <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -869,18 +861,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10001</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -889,18 +881,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10002</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -909,18 +901,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10003</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>32</v>
@@ -932,206 +924,206 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10004</v>
       </c>
       <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10005</v>
       </c>
       <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>10006</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
         <v>52</v>
       </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10007</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="114" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10008</v>
       </c>
       <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10009</v>
       </c>
       <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
         <v>62</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>63</v>
       </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
       <c r="E11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10010</v>
       </c>
       <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>66</v>
       </c>
-      <c r="E12" t="s">
-        <v>67</v>
-      </c>
       <c r="F12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10011</v>
       </c>
       <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
         <v>94</v>
       </c>
-      <c r="C13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>95</v>
       </c>
-      <c r="E13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10012</v>
       </c>
       <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>69</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10013</v>
       </c>
       <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
         <v>72</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="128.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10014</v>
       </c>
       <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
         <v>77</v>
       </c>
-      <c r="C16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -1139,16 +1131,16 @@
         <v>10015</v>
       </c>
       <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
         <v>80</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>81</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="185.25" x14ac:dyDescent="0.2">
@@ -1156,16 +1148,16 @@
         <v>10016</v>
       </c>
       <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
         <v>84</v>
       </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1173,16 +1165,16 @@
         <v>10017</v>
       </c>
       <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" t="s">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" t="s">
-        <v>88</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1190,22 +1182,22 @@
         <v>10018</v>
       </c>
       <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" t="s">
         <v>89</v>
       </c>
-      <c r="C20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" t="s">
-        <v>91</v>
-      </c>
       <c r="G20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1218,16 +1210,16 @@
         <v>20001</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>